<commit_message>
v8.5: multiple wireless trailer support and much more. See change log
</commit_message>
<xml_diff>
--- a/documentation/adjustmentsRemote.xlsx
+++ b/documentation/adjustmentsRemote.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168B8D9E-B71E-3A45-8A5C-758DDBE9C2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E2372C-C43C-7C41-8FCC-3A06C02D4B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="1380" windowWidth="46720" windowHeight="24940" xr2:uid="{7FD8C6E5-3068-1C47-BC39-03FF60370E8F}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
   <si>
     <t>up</t>
   </si>
@@ -407,12 +407,15 @@
   <si>
     <t>(3 = not in PWM communication mode. Connect servo to CH4 header</t>
   </si>
+  <si>
+    <t>Horn, bluelight &amp; siren / winch / trailer legs / trailer ramps</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -444,6 +447,13 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Textkörper)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -694,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -731,6 +741,147 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -767,155 +918,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1286,7 +1299,7 @@
   <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E20"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1312,68 +1325,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
-      <c r="I1" s="36" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="I1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="P1" s="48" t="s">
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="P1" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="39" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47" t="s">
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="P2" s="47" t="s">
+      <c r="N2" s="56"/>
+      <c r="P2" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47" t="s">
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="47"/>
+      <c r="U2" s="56"/>
     </row>
     <row r="3" spans="1:21" ht="32" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1388,9 +1401,9 @@
       <c r="D3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="40"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="21"/>
       <c r="I3" s="10" t="s">
         <v>77</v>
       </c>
@@ -1429,19 +1442,19 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="38" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="11">
@@ -1458,10 +1471,10 @@
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="28"/>
+      <c r="N4" s="37"/>
       <c r="P4" s="4">
         <v>1</v>
       </c>
@@ -1470,17 +1483,17 @@
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="28" t="s">
+      <c r="T4" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="28"/>
+      <c r="U4" s="37"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="52"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="11">
         <v>2</v>
       </c>
@@ -1495,10 +1508,10 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="28"/>
+      <c r="N5" s="37"/>
       <c r="P5" s="4">
         <v>2</v>
       </c>
@@ -1507,17 +1520,17 @@
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="28" t="s">
+      <c r="T5" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="28"/>
+      <c r="U5" s="37"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="52"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="11">
         <v>3</v>
       </c>
@@ -1532,10 +1545,10 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="28"/>
+      <c r="N6" s="37"/>
       <c r="P6" s="4">
         <v>3</v>
       </c>
@@ -1544,17 +1557,17 @@
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="28" t="s">
+      <c r="T6" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="U6" s="28"/>
+      <c r="U6" s="37"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="65"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="52"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="11">
         <v>4</v>
       </c>
@@ -1569,10 +1582,10 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" s="28"/>
+      <c r="M7" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="N7" s="78"/>
       <c r="P7" s="4">
         <v>5</v>
       </c>
@@ -1581,30 +1594,30 @@
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="28" t="s">
+      <c r="T7" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="U7" s="28"/>
+      <c r="U7" s="37"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="65"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="41">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="60">
         <v>5</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="46">
         <v>2</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K8" s="50" t="s">
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1616,13 +1629,13 @@
       <c r="N8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="30">
+      <c r="P8" s="46">
         <v>4</v>
       </c>
-      <c r="Q8" s="33" t="s">
+      <c r="Q8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="R8" s="31" t="s">
+      <c r="R8" s="50" t="s">
         <v>12</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -1636,70 +1649,70 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="65"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="45"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="31"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="53"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="50"/>
       <c r="L9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="32"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="31"/>
+      <c r="N9" s="51"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="50"/>
       <c r="S9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="32"/>
+      <c r="U9" s="51"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="65"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="45"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="31"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="53"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="50"/>
       <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="32"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="31"/>
+      <c r="N10" s="51"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="50"/>
       <c r="S10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U10" s="32"/>
+      <c r="U10" s="51"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="65"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="45"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="31" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="53"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="50" t="s">
         <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -1711,9 +1724,9 @@
       <c r="N11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="31" t="s">
+      <c r="P11" s="46"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="50" t="s">
         <v>13</v>
       </c>
       <c r="S11" s="1" t="s">
@@ -1727,78 +1740,78 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="65"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="45"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="31"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="53"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="50"/>
       <c r="L12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="32"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="31"/>
+      <c r="N12" s="51"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="50"/>
       <c r="S12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T12" s="1"/>
-      <c r="U12" s="32"/>
+      <c r="U12" s="51"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="65"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="46"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="31"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="54"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
       <c r="L13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="32"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="31"/>
+      <c r="N13" s="51"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="50"/>
       <c r="S13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U13" s="32"/>
+      <c r="U13" s="51"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="41">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="60">
         <v>6</v>
       </c>
-      <c r="G14" s="44" t="s">
+      <c r="G14" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I14" s="46">
         <v>4</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="J14" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="K14" s="50" t="s">
         <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1808,11 +1821,11 @@
       <c r="N14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="55">
+      <c r="P14" s="41">
         <v>16</v>
       </c>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="55"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="41"/>
       <c r="S14" s="6" t="s">
         <v>5</v>
       </c>
@@ -1820,68 +1833,68 @@
       <c r="U14" s="6"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="45"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="31"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="53"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="50"/>
       <c r="L15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="32"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="55"/>
+      <c r="N15" s="51"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="41"/>
       <c r="S15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T15" s="6"/>
-      <c r="U15" s="59"/>
+      <c r="U15" s="45"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="65"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="45"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="31"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="53"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="50"/>
       <c r="L16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="32"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="55"/>
+      <c r="N16" s="51"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="41"/>
       <c r="S16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T16" s="6"/>
-      <c r="U16" s="59"/>
+      <c r="U16" s="45"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="45"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="31" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="53"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="50" t="s">
         <v>13</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1891,9 +1904,9 @@
       <c r="N17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="57"/>
-      <c r="R17" s="55"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="41"/>
       <c r="S17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1901,65 +1914,65 @@
       <c r="U17" s="6"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="45"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="31"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="53"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="50"/>
       <c r="L18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N18" s="32"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="57"/>
-      <c r="R18" s="55"/>
+      <c r="N18" s="51"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="41"/>
       <c r="S18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T18" s="6"/>
-      <c r="U18" s="59"/>
+      <c r="U18" s="45"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="65"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="46"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="31"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="54"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="50"/>
       <c r="L19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="32"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="55"/>
+      <c r="N19" s="51"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="44"/>
+      <c r="R19" s="41"/>
       <c r="S19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T19" s="6"/>
-      <c r="U19" s="59"/>
+      <c r="U19" s="45"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="52"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="11">
         <v>7</v>
       </c>
@@ -1974,27 +1987,27 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="29" t="s">
+      <c r="M20" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="N20" s="29"/>
+      <c r="N20" s="75"/>
       <c r="P20" s="7">
         <v>16</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="49" t="s">
+      <c r="T20" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="U20" s="49"/>
+      <c r="U20" s="34"/>
     </row>
     <row r="21" spans="1:21" ht="16" customHeight="1">
-      <c r="A21" s="67"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="53" t="s">
+      <c r="A21" s="27"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="39" t="s">
         <v>59</v>
       </c>
       <c r="F21" s="11">
@@ -2011,10 +2024,10 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="28" t="s">
+      <c r="M21" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="N21" s="28"/>
+      <c r="N21" s="37"/>
       <c r="P21" s="4">
         <v>6</v>
       </c>
@@ -2023,19 +2036,19 @@
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="28" t="s">
+      <c r="T21" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="U21" s="28"/>
+      <c r="U21" s="37"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="67"/>
-      <c r="B22" s="66" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="54"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="11">
         <v>9</v>
       </c>
@@ -2050,10 +2063,10 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="50" t="s">
+      <c r="M22" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="N22" s="51"/>
+      <c r="N22" s="33"/>
       <c r="P22" s="4">
         <v>7</v>
       </c>
@@ -2062,16 +2075,16 @@
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="50" t="s">
+      <c r="T22" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="U22" s="51"/>
+      <c r="U22" s="33"/>
     </row>
     <row r="23" spans="1:21" ht="17">
-      <c r="A23" s="67"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="12" t="s">
         <v>7</v>
       </c>
@@ -2087,10 +2100,10 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="49" t="s">
+      <c r="M23" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="N23" s="49"/>
+      <c r="N23" s="34"/>
       <c r="P23" s="4">
         <v>8</v>
       </c>
@@ -2099,17 +2112,17 @@
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="50" t="s">
+      <c r="T23" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="U23" s="51"/>
+      <c r="U23" s="33"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="67"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="69" t="s">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="29" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="11">
@@ -2124,10 +2137,10 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="49" t="s">
+      <c r="M24" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="49"/>
+      <c r="N24" s="34"/>
       <c r="P24" s="4">
         <v>9</v>
       </c>
@@ -2136,17 +2149,17 @@
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="50" t="s">
+      <c r="T24" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="U24" s="51"/>
+      <c r="U24" s="33"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="67"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="70"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="11">
         <v>12</v>
       </c>
@@ -2159,10 +2172,10 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="49" t="s">
+      <c r="M25" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="49"/>
+      <c r="N25" s="34"/>
       <c r="P25" s="4">
         <v>10</v>
       </c>
@@ -2171,17 +2184,17 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="60" t="s">
+      <c r="T25" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="U25" s="61"/>
+      <c r="U25" s="36"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="68"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="71"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="11">
         <v>13</v>
       </c>
@@ -2194,10 +2207,10 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="49" t="s">
+      <c r="M26" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="N26" s="49"/>
+      <c r="N26" s="34"/>
       <c r="P26" s="4">
         <v>11</v>
       </c>
@@ -2206,208 +2219,208 @@
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="60" t="s">
+      <c r="T26" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="U26" s="61"/>
+      <c r="U26" s="36"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="I28" s="73" t="s">
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="I28" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="73"/>
-      <c r="M28" s="73"/>
-      <c r="N28" s="73"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
       <c r="P28" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="75" t="s">
+      <c r="A29" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="I29" s="72" t="s">
+      <c r="B29" s="77"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="I29" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="73"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="76" t="s">
+      <c r="A30" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="I30" s="73"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="73"/>
-      <c r="N30" s="73"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
     </row>
     <row r="31" spans="1:21" ht="16" customHeight="1">
-      <c r="I31" s="77" t="s">
+      <c r="I31" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="77"/>
-      <c r="N31" s="77"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="1:21" ht="16" customHeight="1">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21"/>
-      <c r="I32" s="77"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="68"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
     </row>
     <row r="33" spans="1:14" ht="16" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="24"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
     </row>
     <row r="34" spans="1:14" ht="16" customHeight="1">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
-      <c r="I34" s="77" t="s">
+      <c r="A34" s="69"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
+      <c r="I34" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
-      <c r="N34" s="77"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="22"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="24"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="77"/>
-      <c r="L35" s="77"/>
-      <c r="M35" s="77"/>
-      <c r="N35" s="77"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="22"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="24"/>
-      <c r="I36" s="73" t="s">
+      <c r="A36" s="69"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71"/>
+      <c r="I36" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
-      <c r="M36" s="73"/>
-      <c r="N36" s="73"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="22"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="24"/>
-      <c r="I37" s="72" t="s">
+      <c r="A37" s="69"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="71"/>
+      <c r="I37" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="J37" s="72"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="72"/>
-      <c r="M37" s="72"/>
-      <c r="N37" s="72"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="22"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="24"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="72"/>
-      <c r="N38" s="72"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="71"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
     </row>
     <row r="39" spans="1:14" ht="16" customHeight="1">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="27"/>
-      <c r="I39" s="16" t="s">
+      <c r="A39" s="72"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="74"/>
+      <c r="I39" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="18"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="64"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="64"/>
+      <c r="N39" s="65"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="13"/>
@@ -2438,27 +2451,50 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="I28:N28"/>
-    <mergeCell ref="I29:N30"/>
-    <mergeCell ref="I31:N33"/>
-    <mergeCell ref="I34:N35"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:A19"/>
-    <mergeCell ref="B4:B21"/>
-    <mergeCell ref="C4:C26"/>
-    <mergeCell ref="D4:D26"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="I39:N39"/>
+    <mergeCell ref="A32:G39"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="I14:I19"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="J14:J19"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="I37:N38"/>
+    <mergeCell ref="I36:N36"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="F14:F19"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N12:N13"/>
     <mergeCell ref="T21:U21"/>
     <mergeCell ref="T20:U20"/>
     <mergeCell ref="T22:U22"/>
@@ -2475,50 +2511,27 @@
     <mergeCell ref="T7:U7"/>
     <mergeCell ref="P8:P13"/>
     <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="F14:F19"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="I39:N39"/>
-    <mergeCell ref="A32:G39"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="I14:I19"/>
-    <mergeCell ref="K14:K16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="J14:J19"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="I37:N38"/>
-    <mergeCell ref="I36:N36"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:A19"/>
+    <mergeCell ref="B4:B21"/>
+    <mergeCell ref="C4:C26"/>
+    <mergeCell ref="D4:D26"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="I28:N28"/>
+    <mergeCell ref="I29:N30"/>
+    <mergeCell ref="I31:N33"/>
+    <mergeCell ref="I34:N35"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
v9.0: AIRPLANE_MODE, trailer ramps ESC mode
</commit_message>
<xml_diff>
--- a/documentation/adjustmentsRemote.xlsx
+++ b/documentation/adjustmentsRemote.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E2372C-C43C-7C41-8FCC-3A06C02D4B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C64AEE-FFC0-454D-AC33-C2A3E5860A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="1380" windowWidth="46720" windowHeight="24940" xr2:uid="{7FD8C6E5-3068-1C47-BC39-03FF60370E8F}"/>
+    <workbookView xWindow="5180" yWindow="1420" windowWidth="46720" windowHeight="24940" xr2:uid="{7FD8C6E5-3068-1C47-BC39-03FF60370E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -741,194 +741,194 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -985,6 +985,50 @@
         <a:xfrm>
           <a:off x="11651141" y="5948679"/>
           <a:ext cx="3113879" cy="3105325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>853440</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>134551</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B68745-487F-E548-8CE8-3143DD8C668E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="436880" y="8351520"/>
+          <a:ext cx="7772400" cy="3578791"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1298,8 +1342,8 @@
   </sheetPr>
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1325,68 +1369,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
-      <c r="I1" s="57" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="69"/>
+      <c r="I1" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="P1" s="55" t="s">
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="P1" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="20" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56" t="s">
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="56"/>
-      <c r="P2" s="56" t="s">
+      <c r="N2" s="55"/>
+      <c r="P2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56" t="s">
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="56"/>
+      <c r="U2" s="55"/>
     </row>
     <row r="3" spans="1:21" ht="32" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1401,9 +1445,9 @@
       <c r="D3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="21"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="47"/>
       <c r="I3" s="10" t="s">
         <v>77</v>
       </c>
@@ -1442,19 +1486,19 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="57" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="11">
@@ -1471,10 +1515,10 @@
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="37"/>
+      <c r="N4" s="28"/>
       <c r="P4" s="4">
         <v>1</v>
       </c>
@@ -1483,17 +1527,17 @@
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="37" t="s">
+      <c r="T4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="37"/>
+      <c r="U4" s="28"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="38"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="11">
         <v>2</v>
       </c>
@@ -1508,10 +1552,10 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="37" t="s">
+      <c r="M5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="37"/>
+      <c r="N5" s="28"/>
       <c r="P5" s="4">
         <v>2</v>
       </c>
@@ -1520,17 +1564,17 @@
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="37" t="s">
+      <c r="T5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="37"/>
+      <c r="U5" s="28"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="38"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="11">
         <v>3</v>
       </c>
@@ -1545,10 +1589,10 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="37" t="s">
+      <c r="M6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="37"/>
+      <c r="N6" s="28"/>
       <c r="P6" s="4">
         <v>3</v>
       </c>
@@ -1557,17 +1601,17 @@
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="37" t="s">
+      <c r="T6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="U6" s="37"/>
+      <c r="U6" s="28"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="38"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="57"/>
       <c r="F7" s="11">
         <v>4</v>
       </c>
@@ -1582,10 +1626,10 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="78" t="s">
+      <c r="M7" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="N7" s="78"/>
+      <c r="N7" s="54"/>
       <c r="P7" s="4">
         <v>5</v>
       </c>
@@ -1594,30 +1638,30 @@
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="37" t="s">
+      <c r="T7" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="U7" s="37"/>
+      <c r="U7" s="28"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="60">
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="48">
         <v>5</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="46">
+      <c r="I8" s="30">
         <v>2</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="50" t="s">
+      <c r="K8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1629,13 +1673,13 @@
       <c r="N8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="46">
+      <c r="P8" s="30">
         <v>4</v>
       </c>
-      <c r="Q8" s="47" t="s">
+      <c r="Q8" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="R8" s="50" t="s">
+      <c r="R8" s="31" t="s">
         <v>12</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -1649,70 +1693,70 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="53"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="50"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="52"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="51"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="50"/>
+      <c r="N9" s="32"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="31"/>
       <c r="S9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="51"/>
+      <c r="U9" s="32"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="53"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="50"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="52"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="51"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="50"/>
+      <c r="N10" s="32"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="31"/>
       <c r="S10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U10" s="51"/>
+      <c r="U10" s="32"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="53"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="50" t="s">
+      <c r="A11" s="70"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="52"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="31" t="s">
         <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -1724,9 +1768,9 @@
       <c r="N11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="50" t="s">
+      <c r="P11" s="30"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="31" t="s">
         <v>13</v>
       </c>
       <c r="S11" s="1" t="s">
@@ -1740,78 +1784,78 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="53"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="50"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="52"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="31"/>
       <c r="L12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="51"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="50"/>
+      <c r="N12" s="32"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="31"/>
       <c r="S12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T12" s="1"/>
-      <c r="U12" s="51"/>
+      <c r="U12" s="32"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="54"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="50"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="53"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="31"/>
       <c r="L13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="51"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="50"/>
+      <c r="N13" s="32"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="31"/>
       <c r="S13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U13" s="51"/>
+      <c r="U13" s="32"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="60">
+      <c r="A14" s="70"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="48">
         <v>6</v>
       </c>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="46">
+      <c r="I14" s="30">
         <v>4</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="50" t="s">
+      <c r="K14" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1821,11 +1865,11 @@
       <c r="N14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="41">
+      <c r="P14" s="60">
         <v>16</v>
       </c>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="41"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="60"/>
       <c r="S14" s="6" t="s">
         <v>5</v>
       </c>
@@ -1833,68 +1877,68 @@
       <c r="U14" s="6"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="53"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="50"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="52"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="31"/>
       <c r="L15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="51"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="41"/>
+      <c r="N15" s="32"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="60"/>
       <c r="S15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T15" s="6"/>
-      <c r="U15" s="45"/>
+      <c r="U15" s="64"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="53"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="50"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="52"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="51"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="41"/>
+      <c r="N16" s="32"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="60"/>
       <c r="S16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T16" s="6"/>
-      <c r="U16" s="45"/>
+      <c r="U16" s="64"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="53"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="50" t="s">
+      <c r="A17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="52"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="31" t="s">
         <v>13</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1904,9 +1948,9 @@
       <c r="N17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="41"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="60"/>
       <c r="S17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1914,65 +1958,65 @@
       <c r="U17" s="6"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="53"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="50"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="52"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="31"/>
       <c r="L18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N18" s="51"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="41"/>
+      <c r="N18" s="32"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="60"/>
       <c r="S18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T18" s="6"/>
-      <c r="U18" s="45"/>
+      <c r="U18" s="64"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="54"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="50"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="53"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="31"/>
       <c r="L19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="51"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="41"/>
+      <c r="N19" s="32"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="60"/>
       <c r="S19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T19" s="6"/>
-      <c r="U19" s="45"/>
+      <c r="U19" s="64"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="38"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="11">
         <v>7</v>
       </c>
@@ -1987,27 +2031,27 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="75" t="s">
+      <c r="M20" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="N20" s="75"/>
+      <c r="N20" s="29"/>
       <c r="P20" s="7">
         <v>16</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="34" t="s">
+      <c r="T20" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="U20" s="34"/>
+      <c r="U20" s="36"/>
     </row>
     <row r="21" spans="1:21" ht="16" customHeight="1">
-      <c r="A21" s="27"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="39" t="s">
+      <c r="A21" s="72"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="58" t="s">
         <v>59</v>
       </c>
       <c r="F21" s="11">
@@ -2024,10 +2068,10 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="37" t="s">
+      <c r="M21" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="N21" s="37"/>
+      <c r="N21" s="28"/>
       <c r="P21" s="4">
         <v>6</v>
       </c>
@@ -2036,19 +2080,19 @@
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="37" t="s">
+      <c r="T21" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="U21" s="37"/>
+      <c r="U21" s="28"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="27"/>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="72"/>
+      <c r="B22" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="40"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="59"/>
       <c r="F22" s="11">
         <v>9</v>
       </c>
@@ -2063,10 +2107,10 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="32" t="s">
+      <c r="M22" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="N22" s="33"/>
+      <c r="N22" s="38"/>
       <c r="P22" s="4">
         <v>7</v>
       </c>
@@ -2075,16 +2119,16 @@
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="32" t="s">
+      <c r="T22" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="U22" s="33"/>
+      <c r="U22" s="38"/>
     </row>
     <row r="23" spans="1:21" ht="17">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
       <c r="E23" s="12" t="s">
         <v>7</v>
       </c>
@@ -2100,10 +2144,10 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="34" t="s">
+      <c r="M23" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="N23" s="34"/>
+      <c r="N23" s="36"/>
       <c r="P23" s="4">
         <v>8</v>
       </c>
@@ -2112,17 +2156,17 @@
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="32" t="s">
+      <c r="T23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="U23" s="33"/>
+      <c r="U23" s="38"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="29" t="s">
+      <c r="A24" s="72"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="74" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="11">
@@ -2137,10 +2181,10 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="34" t="s">
+      <c r="M24" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="34"/>
+      <c r="N24" s="36"/>
       <c r="P24" s="4">
         <v>9</v>
       </c>
@@ -2149,17 +2193,17 @@
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="32" t="s">
+      <c r="T24" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="U24" s="33"/>
+      <c r="U24" s="38"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="30"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="75"/>
       <c r="F25" s="11">
         <v>12</v>
       </c>
@@ -2172,10 +2216,10 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="34"/>
+      <c r="N25" s="36"/>
       <c r="P25" s="4">
         <v>10</v>
       </c>
@@ -2184,17 +2228,17 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="35" t="s">
+      <c r="T25" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="U25" s="36"/>
+      <c r="U25" s="66"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="28"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="31"/>
+      <c r="A26" s="73"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="76"/>
       <c r="F26" s="11">
         <v>13</v>
       </c>
@@ -2207,10 +2251,10 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="34" t="s">
+      <c r="M26" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="N26" s="34"/>
+      <c r="N26" s="36"/>
       <c r="P26" s="4">
         <v>11</v>
       </c>
@@ -2219,208 +2263,208 @@
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="35" t="s">
+      <c r="T26" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="U26" s="36"/>
+      <c r="U26" s="66"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
-      <c r="I28" s="17" t="s">
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="I28" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
       <c r="P28" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="77"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="I29" s="18" t="s">
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="I29" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
     </row>
     <row r="31" spans="1:21" ht="16" customHeight="1">
-      <c r="I31" s="19" t="s">
+      <c r="I31" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
+      <c r="J31" s="78"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="78"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="78"/>
     </row>
     <row r="32" spans="1:21" ht="16" customHeight="1">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="I32" s="78"/>
+      <c r="J32" s="78"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="78"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="78"/>
     </row>
     <row r="33" spans="1:14" ht="16" customHeight="1">
-      <c r="A33" s="69"/>
-      <c r="B33" s="70"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="71"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
+      <c r="I33" s="78"/>
+      <c r="J33" s="78"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="78"/>
     </row>
     <row r="34" spans="1:14" ht="16" customHeight="1">
-      <c r="A34" s="69"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="71"/>
-      <c r="I34" s="19" t="s">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+      <c r="I34" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="78"/>
+      <c r="M34" s="78"/>
+      <c r="N34" s="78"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="69"/>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="71"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+      <c r="I35" s="78"/>
+      <c r="J35" s="78"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="78"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="78"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="69"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="71"/>
-      <c r="I36" s="17" t="s">
+      <c r="A36" s="22"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="24"/>
+      <c r="I36" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="69"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="71"/>
-      <c r="I37" s="18" t="s">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="24"/>
+      <c r="I37" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="69"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="71"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="24"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39"/>
     </row>
     <row r="39" spans="1:14" ht="16" customHeight="1">
-      <c r="A39" s="72"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="74"/>
-      <c r="I39" s="63" t="s">
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
+      <c r="I39" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J39" s="64"/>
-      <c r="K39" s="64"/>
-      <c r="L39" s="64"/>
-      <c r="M39" s="64"/>
-      <c r="N39" s="65"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="18"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="13"/>
@@ -2451,6 +2495,71 @@
     </row>
   </sheetData>
   <mergeCells count="81">
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="I28:N28"/>
+    <mergeCell ref="I29:N30"/>
+    <mergeCell ref="I31:N33"/>
+    <mergeCell ref="I34:N35"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:A19"/>
+    <mergeCell ref="B4:B21"/>
+    <mergeCell ref="C4:C26"/>
+    <mergeCell ref="D4:D26"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="E4:E20"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="P14:P19"/>
+    <mergeCell ref="Q14:Q19"/>
+    <mergeCell ref="R14:R16"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="R17:R19"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="Q8:Q13"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="F14:F19"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K13"/>
     <mergeCell ref="I39:N39"/>
     <mergeCell ref="A32:G39"/>
     <mergeCell ref="M21:N21"/>
@@ -2467,71 +2576,6 @@
     <mergeCell ref="I36:N36"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A29:G29"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="F14:F19"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="G14:G19"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="E4:E20"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="P14:P19"/>
-    <mergeCell ref="Q14:Q19"/>
-    <mergeCell ref="R14:R16"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="R17:R19"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:A19"/>
-    <mergeCell ref="B4:B21"/>
-    <mergeCell ref="C4:C26"/>
-    <mergeCell ref="D4:D26"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="I28:N28"/>
-    <mergeCell ref="I29:N30"/>
-    <mergeCell ref="I31:N33"/>
-    <mergeCell ref="I34:N35"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>